<commit_message>
filling in results and voronoi norm params
Filling in the results table with the tp fp tn fn and the accuracy, precision and recall for ovalb and ca ox

Saving normalised voronoi params in txt file for both caox and alb
</commit_message>
<xml_diff>
--- a/Results summary table.xlsx
+++ b/Results summary table.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/58209e4e11c8586d/Documents/Uni/4th year/MPhys Sem2/Pee-stain-pathology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{50DCB5F4-642F-458E-9072-DC40506D5FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EFF6DDA-073C-4BF9-91BA-AA720920BE33}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="8_{50DCB5F4-642F-458E-9072-DC40506D5FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9BDE857-CCC2-43B2-8A8D-6F2C552FBAFA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E873254C-42DA-4C40-ADBB-08B9C2B2DF68}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{E873254C-42DA-4C40-ADBB-08B9C2B2DF68}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CaOx" sheetId="2" r:id="rId1"/>
+    <sheet name="Ovalbumin" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,29 +37,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Model</t>
   </si>
   <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precision </t>
-  </si>
-  <si>
     <t>Recall</t>
   </si>
   <si>
     <t>NN</t>
   </si>
   <si>
-    <t>CaOx</t>
-  </si>
-  <si>
-    <t>Albumin</t>
-  </si>
-  <si>
     <t>CNN (2) classes</t>
   </si>
   <si>
@@ -74,7 +63,31 @@
     <t>K means</t>
   </si>
   <si>
-    <t>10 epochs</t>
+    <t>Ovalbumin</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>Voronoi log reg</t>
+  </si>
+  <si>
+    <t>Acc</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Calcium oxalate</t>
   </si>
 </sst>
 </file>
@@ -98,18 +111,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -124,10 +131,19 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -140,11 +156,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -160,6 +176,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,11 +478,263 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{768714C9-263C-466F-974B-212051EBB4B8}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L13" sqref="L13:L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.7265625" customWidth="1"/>
+    <col min="8" max="8" width="10.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.3145</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.18540000000000001</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.3826</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.1174</v>
+      </c>
+      <c r="F3" s="1">
+        <f xml:space="preserve"> (B3+D3)/SUM(B3:E3)</f>
+        <v>0.69716971697169716</v>
+      </c>
+      <c r="G3" s="1">
+        <f>B3/(B3+C3)</f>
+        <v>0.62912582516503301</v>
+      </c>
+      <c r="H3" s="1">
+        <f>B3/(B3+E3)</f>
+        <v>0.72817781893956934</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="C4" s="2">
+        <v>8.7900000000000006E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.34289999999999998</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.157</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F9" si="0" xml:space="preserve"> (B4+D4)/SUM(B4:E4)</f>
+        <v>0.75505101020204035</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" ref="G4:G9" si="1">B4/(B4+C4)</f>
+        <v>0.82416483296659326</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H9" si="2">B4/(B4+E4)</f>
+        <v>0.72407732864674867</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H5" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.42759999999999998</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7.2400000000000006E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.37109999999999999</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.12889999999999999</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.79869999999999997</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.85519999999999996</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="2"/>
+        <v>0.7683737646001797</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.20039999999999999</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4.9500000000000002E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.66459999999999997</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.28575715143028607</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.80192076830732284</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="2"/>
+        <v>0.23167630057803468</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.19120000000000001</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5.0799999999999998E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.12709999999999999</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.62290000000000001</v>
+      </c>
+      <c r="F8" s="1">
+        <f xml:space="preserve"> (B8+D8)/SUM(B8:E8)</f>
+        <v>0.32086693548387102</v>
+      </c>
+      <c r="G8" s="1">
+        <f>B8/(B8+C8)</f>
+        <v>0.79008264462809918</v>
+      </c>
+      <c r="H8" s="1">
+        <f>B8/(B8+E8)</f>
+        <v>0.23486058223805428</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.42630000000000001</v>
+      </c>
+      <c r="C9">
+        <v>7.3599999999999999E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.1368</v>
+      </c>
+      <c r="E9">
+        <v>0.36314999999999997</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.56318447767165081</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.85277055411082214</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="2"/>
+        <v>0.53999619988599656</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE930698-D96C-46E6-A5A7-CDFF1C3E4401}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="I9" sqref="I3:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,138 +744,264 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.42780000000000001</v>
+      </c>
+      <c r="C3" s="2">
+        <v>7.22E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.28170000000000001</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.21879999999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <f>(B3+D3)/SUM(B3:E3)</f>
+        <v>0.70914542728635677</v>
+      </c>
+      <c r="G3" s="1">
+        <f>B3/(B3+C3)</f>
+        <v>0.85560000000000003</v>
+      </c>
+      <c r="H3" s="1">
+        <f>B3/(B3+E3)</f>
+        <v>0.66161459944324152</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I8" si="0">SUM(B3:E3)</f>
+        <v>1.0005000000000002</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3">
-        <v>0.89</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.3846</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.1154</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.39860000000000001</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.1013</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F9" si="1">(B4+D4)/SUM(B4:E4)</f>
+        <v>0.78327832783278328</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" ref="G4:G9" si="2">B4/(B4+C4)</f>
+        <v>0.76919999999999999</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H9" si="3">B4/(B4+E4)</f>
+        <v>0.7915208890718255</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0.99990000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
-        <v>9.5000000000000001E-2</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H5" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.43959999999999999</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.433</v>
+      </c>
+      <c r="E6" s="7">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.87382335269377143</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="2"/>
+        <v>0.87990392313851085</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="3"/>
+        <v>0.86946202531645556</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0.99859999999999993</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.16489999999999999</v>
+      </c>
+      <c r="C7" s="2">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.16020000000000001</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.58979999999999999</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.32513251325132514</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="2"/>
+        <v>0.65986394557823125</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="3"/>
+        <v>0.21849741619186433</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0.99990000000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
       <c r="B8" s="2">
-        <v>1</v>
+        <v>0.19040000000000001</v>
       </c>
       <c r="C8" s="2">
-        <v>0.66666000000000003</v>
+        <v>5.45E-2</v>
       </c>
       <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3">
-        <v>1</v>
-      </c>
-      <c r="I8" s="7"/>
+        <v>0.20580000000000001</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.54420000000000002</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.39823097798773743</v>
+      </c>
+      <c r="G8" s="1">
+        <f>B8/(B8+C8)</f>
+        <v>0.77746018783176807</v>
+      </c>
+      <c r="H8" s="1">
+        <f>B8/(B8+E8)</f>
+        <v>0.25918867410835827</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0.99490000000000001</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.41439999999999999</v>
+      </c>
+      <c r="C9">
+        <v>8.5500000000000007E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.25650000000000001</v>
+      </c>
+      <c r="E9">
+        <v>0.24340000000000001</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.67103420684136827</v>
+      </c>
+      <c r="G9" s="1">
+        <f>B9/(B9+C9)</f>
+        <v>0.82896579315863173</v>
+      </c>
+      <c r="H9" s="1">
+        <f>B9/(B9+E9)</f>
+        <v>0.62997871693523877</v>
+      </c>
+      <c r="I9">
+        <f>SUM(B9:E9)</f>
+        <v>0.99980000000000002</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>